<commit_message>
Added peak plot generation
</commit_message>
<xml_diff>
--- a/Data/Sorted_Inactivation/sortingNotes/sortingNotes_20150313_R.xlsx
+++ b/Data/Sorted_Inactivation/sortingNotes/sortingNotes_20150313_R.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\LaboDancauseDS\home\sortedDataMatlabFormat\InactivationData\NewSorting\Notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\14252\NHP Data Analysis\Data\Sorted_Inactivation\sortingNotes\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A00B47-FD97-49A3-A945-9C713093DECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,6 +27,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -89,7 +92,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -528,12 +531,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M257"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J227" sqref="J227"/>
+      <pane ySplit="1" topLeftCell="A232" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E249" sqref="E249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3841,7 +3844,10 @@
         <v>11</v>
       </c>
       <c r="C140">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D140">
+        <v>2</v>
       </c>
       <c r="I140">
         <f t="shared" si="8"/>
@@ -4126,10 +4132,7 @@
         <v>23</v>
       </c>
       <c r="C152">
-        <v>1</v>
-      </c>
-      <c r="D152">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I152">
         <f t="shared" si="9"/>
@@ -6433,7 +6436,7 @@
         <v>121</v>
       </c>
       <c r="C250">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I250">
         <f t="shared" si="15"/>

</xml_diff>